<commit_message>
brows button layout in itmebutton
</commit_message>
<xml_diff>
--- a/viewModel.xlsx
+++ b/viewModel.xlsx
@@ -1756,8 +1756,8 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>40821</xdr:rowOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>68036</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
@@ -1772,60 +1772,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="680357" y="9239250"/>
-          <a:ext cx="13375822" cy="8422821"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>16329</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>557893</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>108858</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="35" name="正方形/長方形 34"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="832757" y="9391650"/>
-          <a:ext cx="10610850" cy="446315"/>
+          <a:off x="680357" y="10150929"/>
+          <a:ext cx="13375822" cy="7511142"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1910,266 +1858,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>81644</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>68036</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="37" name="正方形/長方形 36"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="832757" y="9987644"/>
-          <a:ext cx="1004207" cy="340178"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>560615</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>81644</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>204107</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>68036</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="38" name="正方形/長方形 37"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1921329" y="9987644"/>
-          <a:ext cx="1004207" cy="340178"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>274864</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>81644</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>598714</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>68036</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="39" name="正方形/長方形 38"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2996293" y="9987644"/>
-          <a:ext cx="1004207" cy="340178"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>669471</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>81644</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>312964</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>68036</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="40" name="正方形/長方形 39"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4071257" y="9987644"/>
-          <a:ext cx="1004207" cy="340178"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>370114</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>81644</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>13607</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>68036</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="49" name="正方形/長方形 48"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5132614" y="9987644"/>
-          <a:ext cx="1004207" cy="340178"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>612322</xdr:colOff>
       <xdr:row>58</xdr:row>
@@ -2432,60 +2120,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>669472</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>97972</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="55" name="正方形/長方形 54"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10874829" y="9394372"/>
-          <a:ext cx="544285" cy="432707"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>84365</xdr:colOff>
       <xdr:row>65</xdr:row>
@@ -2494,8 +2128,8 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>149678</xdr:colOff>
-      <xdr:row>98</xdr:row>
-      <xdr:rowOff>40822</xdr:rowOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2505,7 +2139,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11650436" y="11664044"/>
-          <a:ext cx="2106385" cy="5712278"/>
+          <a:ext cx="2106385" cy="5140777"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2539,7 +2173,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:colOff>258536</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>141516</xdr:rowOff>
     </xdr:from>
@@ -2556,62 +2190,10 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12137571" y="11816445"/>
-          <a:ext cx="1428750" cy="416378"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>163286</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>163285</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>503465</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>149679</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="58" name="円/楕円 57"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11729357" y="11838214"/>
-          <a:ext cx="340179" cy="340179"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
+          <a:off x="11824607" y="11816445"/>
+          <a:ext cx="1741714" cy="416378"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -2645,7 +2227,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:colOff>258536</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>141517</xdr:rowOff>
     </xdr:from>
@@ -2662,62 +2244,10 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12137571" y="12347124"/>
-          <a:ext cx="1428750" cy="416378"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>163286</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>163286</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>503465</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>149679</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="60" name="円/楕円 59"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11729357" y="12368893"/>
-          <a:ext cx="340179" cy="340179"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
+          <a:off x="11824607" y="12347124"/>
+          <a:ext cx="1741714" cy="416378"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -2751,7 +2281,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:colOff>258536</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>155124</xdr:rowOff>
     </xdr:from>
@@ -2768,62 +2298,10 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12137571" y="12891410"/>
-          <a:ext cx="1428750" cy="416378"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>163286</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>503465</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>163287</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="62" name="円/楕円 61"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11729357" y="12913179"/>
-          <a:ext cx="340179" cy="340179"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
+          <a:off x="11824607" y="12891410"/>
+          <a:ext cx="1741714" cy="416378"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -2857,7 +2335,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:colOff>258536</xdr:colOff>
       <xdr:row>76</xdr:row>
       <xdr:rowOff>19053</xdr:rowOff>
     </xdr:from>
@@ -2874,62 +2352,10 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12137571" y="13462910"/>
-          <a:ext cx="1428750" cy="416378"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>163286</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>40822</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>503465</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>27215</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="64" name="円/楕円 63"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11729357" y="13484679"/>
-          <a:ext cx="340179" cy="340179"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
+          <a:off x="11824607" y="13462910"/>
+          <a:ext cx="1741714" cy="416378"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -3398,6 +2824,214 @@
         <a:xfrm>
           <a:off x="7663544" y="15438666"/>
           <a:ext cx="3154136" cy="2073728"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>84365</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>326572</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="74" name="正方形/長方形 73"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11650436" y="16957222"/>
+          <a:ext cx="922565" cy="337457"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>587828</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>149679</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="75" name="正方形/長方形 74"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12834257" y="16957222"/>
+          <a:ext cx="922565" cy="337457"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>370114</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>21774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>40820</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>136623</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="76" name="正方形/長方形 75"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1050471" y="18064845"/>
+          <a:ext cx="8515349" cy="5598528"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>522515</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>174174</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>625930</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="77" name="正方形/長方形 76"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1202872" y="18217245"/>
+          <a:ext cx="4185558" cy="3037112"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3720,8 +3354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W76" sqref="W76"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X78" sqref="X78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>